<commit_message>
descw-1283 finalize template styling and aliases
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_6_rpt_CA_ConsultingServiceUtilization-FY-Summary-byPortfolio.xlsx
+++ b/backend/reports/xlsx/Tab_6_rpt_CA_ConsultingServiceUtilization-FY-Summary-byPortfolio.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2575C08B-6BB3-294A-809A-8D64798FC383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9D4941-E182-014E-BB59-232DCB224B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>{#date=d.date}</t>
   </si>
@@ -44,17 +44,23 @@
     <t>{#fy=d.fiscal_year}</t>
   </si>
   <si>
+    <t>{$row.resource_type}</t>
+  </si>
+  <si>
+    <t>{#rows=d.report[i+1]}</t>
+  </si>
+  <si>
     <t>{#row=d.report[i]}</t>
   </si>
   <si>
-    <t>{#rows=d.report[i+1]}</t>
-  </si>
-  <si>
-    <t>{#totals=d.report_totals[i]}</t>
-  </si>
-  <si>
-    <t>Consulting Service Utilization by Portfolio 
-for {$fy} as of {$date}</t>
+    <t>{$row.total}</t>
+  </si>
+  <si>
+    <t>{$rows}</t>
+  </si>
+  <si>
+    <t>Consulting Service Utilization by Portfolio
+for FY  ({$fy})  as of {$date}</t>
   </si>
   <si>
     <t>Resource Type</t>
@@ -81,19 +87,16 @@
     <t>Total</t>
   </si>
   <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>{$rows}</t>
-  </si>
-  <si>
-    <t>{$row.resource_type}</t>
+    <t>{$row.bcf}</t>
   </si>
   <si>
     <t>BCF</t>
   </si>
   <si>
-    <t>{$row.bcf}</t>
+    <t>DES</t>
+  </si>
+  <si>
+    <t>GC</t>
   </si>
   <si>
     <t>{$row.oss}</t>
@@ -102,9 +105,6 @@
     <t>{$row.des}</t>
   </si>
   <si>
-    <t>DES</t>
-  </si>
-  <si>
     <t>{$row.dp}</t>
   </si>
   <si>
@@ -120,15 +120,9 @@
     <t>{$row.ce}</t>
   </si>
   <si>
-    <t>GC</t>
-  </si>
-  <si>
     <t>{$row.gc}</t>
   </si>
   <si>
-    <t>{$row.total}</t>
-  </si>
-  <si>
     <t>{$totals.bcf}</t>
   </si>
   <si>
@@ -157,13 +151,16 @@
   </si>
   <si>
     <t>{$totals.total}</t>
+  </si>
+  <si>
+    <t>{#totals=d.totals}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -176,12 +173,17 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
+      <b/>
+      <sz val="9"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
       <sz val="18"/>
       <color theme="0"/>
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="BCSans-Regular"/>
     </font>
@@ -191,27 +193,23 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="BCSans-Regular"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="BCSans-Regular"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="BCSans-Regular"/>
     </font>
   </fonts>
   <fills count="4">
@@ -229,17 +227,28 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FFD9D9D9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -257,95 +266,66 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,7 +334,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFBFBFBF"/>
+      <color rgb="FFD9D9D9"/>
       <color rgb="FF003365"/>
       <color rgb="FFC5DAF1"/>
     </mruColors>
@@ -380,8 +360,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>594537</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2411614</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>680356</xdr:rowOff>
     </xdr:to>
@@ -725,200 +705,206 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="9" width="15.83203125" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="38.5" customWidth="1"/>
+    <col min="2" max="11" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="79" customHeight="1" thickBot="1">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="12" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="60" customHeight="1">
+      <c r="A1" s="3"/>
+      <c r="B1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="23" customHeight="1" thickBot="1">
+      <c r="A2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-    </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="9" t="s">
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+    </row>
+    <row r="5" spans="1:11" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A5" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="C5" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:16" ht="17" thickBot="1">
-      <c r="A4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:16" ht="17" thickBot="1">
-      <c r="A5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="14" t="s">
+      <c r="D5" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="E5" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="F5" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="G5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="H5" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="I5" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="J5" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="K5" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="14" t="s">
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="19">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="21">
+      <c r="A7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" ht="21">
+      <c r="A8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="21">
+      <c r="A9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="17">
-      <c r="B9" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="17">
-      <c r="B10" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="17">
-      <c r="B11" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="17">
-      <c r="B12" s="8"/>
-    </row>
-    <row r="13" spans="1:16" ht="17">
-      <c r="B13" s="8" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="21">
+      <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="17">
-      <c r="B14" s="8" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" ht="21">
+      <c r="A11" s="8" t="s">
         <v>0</v>
       </c>
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" ht="19">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" ht="19">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" ht="19">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" ht="19">
+      <c r="B15" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:G1"/>
+  <mergeCells count="1">
+    <mergeCell ref="B1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>